<commit_message>
Ajout de commentaire pour plan de test
</commit_message>
<xml_diff>
--- a/plan de tests/Plan de tests -  Application Orinoco.xlsx
+++ b/plan de tests/Plan de tests -  Application Orinoco.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -56,12 +56,51 @@
   <si>
     <t>La valeur retournée pourrait être érronée (0 au lieu de 1;  et 1 au lieu de 0)</t>
   </si>
+  <si>
+    <t>index.js</t>
+  </si>
+  <si>
+    <t>panier.js</t>
+  </si>
+  <si>
+    <t>confirmation.js</t>
+  </si>
+  <si>
+    <t>info.js</t>
+  </si>
+  <si>
+    <t>fetch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction Fetch doit récupérer les données présente sur le serveur à l'adresse http://localhost:3000/api/teddies </t>
+  </si>
+  <si>
+    <t>Tester la fonction fetch avec la fonction res et la fonction err. Un console.log(err) est lancé si la connexion au serveur ne s'est pas faite et que les données n'ont pas été récupérées correctement.</t>
+  </si>
+  <si>
+    <t>13 à 96</t>
+  </si>
+  <si>
+    <t>infos</t>
+  </si>
+  <si>
+    <t>La fonction infos doit appeler les données présente dans le serveur  "http://localhost:3000/api/teddies/"+id" , et récupérer celles correspondant à l'id récupéré préalablement dans le code.</t>
+  </si>
+  <si>
+    <t>Afficher le contenu du tableau correspondant à l'id dans la console avec un console.log(infos);</t>
+  </si>
+  <si>
+    <t>Les données du serveur pourraient ne pas s'afficher et la page du site serait vide.</t>
+  </si>
+  <si>
+    <t>Les données récupérés par la fonction pourraient être différentes de celles affichées sur la page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -81,8 +120,20 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +146,12 @@
         <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -105,10 +162,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,15 +181,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -339,11 +407,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -401,90 +469,130 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:26" s="8" customFormat="1" ht="61.5" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:26" ht="26.25" customHeight="1">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" ht="61.5" customHeight="1">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="4:6" ht="26.25" customHeight="1">
       <c r="D17" s="4"/>
@@ -506,7 +614,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="4:6" ht="25.5" customHeight="1">
+    <row r="21" spans="4:6" ht="26.25" customHeight="1">
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -631,7 +739,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="4:6" ht="12">
+    <row r="46" spans="4:6" ht="25.5" customHeight="1">
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -5401,8 +5509,14 @@
       <c r="E999" s="4"/>
       <c r="F999" s="4"/>
     </row>
+    <row r="1000" spans="4:6" ht="12">
+      <c r="D1000" s="4"/>
+      <c r="E1000" s="4"/>
+      <c r="F1000" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Modification et ajout de commentaires divers sur les fichiers javascript
</commit_message>
<xml_diff>
--- a/plan de tests/Plan de tests -  Application Orinoco.xlsx
+++ b/plan de tests/Plan de tests -  Application Orinoco.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve">La fonction Fetch doit récupérer les données présente sur le serveur à l'adresse http://localhost:3000/api/teddies </t>
   </si>
   <si>
-    <t>13 à 96</t>
-  </si>
-  <si>
     <t>infos</t>
   </si>
   <si>
@@ -72,30 +69,15 @@
     <t>Les données récupérés par la fonction pourraient être différentes de celles affichées sur la page.</t>
   </si>
   <si>
-    <t>Chaque ours doit se présenter sous forme de carte avec la photo, le nom, la description, le prix</t>
-  </si>
-  <si>
-    <t>1 à 3</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>18 à 50</t>
-  </si>
-  <si>
     <t>intégration html / variable newInfos</t>
   </si>
   <si>
     <t>Fonction ou variable testée</t>
   </si>
   <si>
-    <t>Récupération de l'id correspondant à l'ours que l'utilisateur a choisi en cliquant sur une carte dans la page d'accueil</t>
-  </si>
-  <si>
-    <t>Tester la fonction Fetch avec la fonction res et la fonction err. Un console.log(err) est lancé si la connexion au serveur ne s'est pas faite et que les données n'ont pas été récupérées correctement.</t>
-  </si>
-  <si>
     <t>L'affichage sur la page Info.html correspond bien aux données récoltées</t>
   </si>
   <si>
@@ -108,12 +90,6 @@
     <t>L'utilisateur n'a pas spécifié de couleur pour son ours et arrive à l'ajouter au panier</t>
   </si>
   <si>
-    <t>68 à 73</t>
-  </si>
-  <si>
-    <t>75 à 80</t>
-  </si>
-  <si>
     <t>quantiteProduit</t>
   </si>
   <si>
@@ -127,9 +103,6 @@
   </si>
   <si>
     <t>monPanier</t>
-  </si>
-  <si>
-    <t>88 à 119</t>
   </si>
   <si>
     <t>Vérifier dans la partie Application de l'inspecteur du navigateur, que le localstorage contient bien les différents produits sélectionnés dans le tableau "monPanier".</t>
@@ -298,20 +271,131 @@
     <t>fetch / POST jsonBody</t>
   </si>
   <si>
+    <t>localstorage</t>
+  </si>
+  <si>
+    <t>Les anciennes informations de l'utilisateur ne sont pas effacées et remplacer par les nouvelles à la reception de l'orderId. Le message de la page de confirmation risque de ne pas récapituler les bonnes informations données par l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Le contenu de "mesInfos" dans le localstorage est effacé et les nouvelles informations nécessaires au message de confirmation y sont stockées.</t>
+  </si>
+  <si>
+    <t>Vérifier dans la partie Application de l'inspecteur du navigateur, que le localstorage contient bien les différents informations de l'utilisateur dans le tableau "mesInfos".</t>
+  </si>
+  <si>
     <t>- Tester la fonction Fetch avec la fonction res et la fonction err. Un console.log(err) est lancé si la connexion au serveur ne s'est pas faite et que les données n'ont pas été récupérées correctement. 
-- Un console log affiche dans la console la valeur récupérée par le serveur (value).</t>
-  </si>
-  <si>
-    <t>localstorage</t>
-  </si>
-  <si>
-    <t>Les anciennes informations de l'utilisateur ne sont pas effacées et remplacer par les nouvelles à la reception de l'orderId. Le message de la page de confirmation risque de ne pas récapituler les bonnes informations données par l'utilisateur.</t>
-  </si>
-  <si>
-    <t>Le contenu de "mesInfos" dans le localstorage est effacé et les nouvelles informations nécessaires au message de confirmation y sont stockées.</t>
-  </si>
-  <si>
-    <t>Vérifier dans la partie Application de l'inspecteur du navigateur, que le localstorage contient bien les différents informations de l'utilisateur dans le tableau "mesInfos".</t>
+- Un console log affiche dans la console la valeur récupérée par le serveur (value).
+- Un console log erreur affiche un message d'erreur si le lien avec le serveur ne se fait pas correctement.</t>
+  </si>
+  <si>
+    <t>La récupération des données contenues dans le localstorage ne se fait pas correctement et n'alimentera pas correctement l'affichage de la page confirmation.html</t>
+  </si>
+  <si>
+    <t>userInfos</t>
+  </si>
+  <si>
+    <t>Le contenu du tableau mesInfos stocké dans le localstorage est récupéré dans une variable appelé "userInfos".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un console.log affiche dans la console le contenu entier de la variable "userInfos". </t>
+  </si>
+  <si>
+    <t>5 à 30</t>
+  </si>
+  <si>
+    <t>intégration html / variables mailConfirmation et infosPerso</t>
+  </si>
+  <si>
+    <t>Le code html, créant un message de confirmation reprenant l'adresse email renseigné par l'utilisateur ainsi qu'un tableau récapitulant les données personnelles récoltées dans la variable userInfos, s'ajoute correctement sur la page confirmation.html.</t>
+  </si>
+  <si>
+    <t>Vérification à l'affichage de la page confirmation.html que l'on retrouve bien les bonnes informations contenus dans la variable userInfos (visible dans la console).</t>
+  </si>
+  <si>
+    <t>Le code html ne s'affiche pas correctement au chargement de la page.</t>
+  </si>
+  <si>
+    <t>Le contenu du tableau monPanier stocké dans le localstorage est récupéré dans une variable appelé "articles".</t>
+  </si>
+  <si>
+    <t>articles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un console.log affiche dans la console le contenu entier de la variable "articles". </t>
+  </si>
+  <si>
+    <t>36 à 71</t>
+  </si>
+  <si>
+    <t>intégration html / variables newLigne et newPrice</t>
+  </si>
+  <si>
+    <t>Le code html, créant un tableau récapitulant les informations des différents articles commandés par l'utilisateur et calculant un prix total des achats, s'ajoute correctement sur la page confirmation.html</t>
+  </si>
+  <si>
+    <t>Vérification à l'affichage de la page confirmation.html que l'on retrouve bien les bonnes informations contenus dans la variable "articles" (visible dans la console).</t>
+  </si>
+  <si>
+    <t>Le tableau monPanier stocké dans le localstorage est supprimé lorsque l'utilisateur a pu confirmé sa commande et a pu arrivé sur la page de confirmation.</t>
+  </si>
+  <si>
+    <t>Vérification à l'affichage en retournant sur la page panier.html que le contenu du panier est vide. Vérifier dans l'inspecteur partie Application que le contenu du localstorage ne contient plus de tableau monPanier.</t>
+  </si>
+  <si>
+    <t>Après confirmation de son achat, le panier de l'utilisateur n'est pas vidé et prêt pour une nouvelle commande.</t>
+  </si>
+  <si>
+    <t>intégration html / variable newElt</t>
+  </si>
+  <si>
+    <t>A l'affichage de la page index.html, chaque ours doit se présenter sous forme de carte avec la photo, le nom, la description, le prix.</t>
+  </si>
+  <si>
+    <t>Récupération de l'id correspondant à l'ours que l'utilisateur a choisi en cliquant sur une carte dans la page d'accueil.</t>
+  </si>
+  <si>
+    <t>Un console.log affiche la valeur de l'id. Vérification à l'affichage de la page, si les infos et la photo de l'ours sont bien celles sur laquelle l'utilisateur a cliqué précédemment.</t>
+  </si>
+  <si>
+    <t>L'id ne se récupère pas, l'url de la page n'intègre pas l'id et donc ne s'affiche correctement.</t>
+  </si>
+  <si>
+    <t>- Tester la fonction Fetch avec la fonction res et la fonction err. 
+- Un console.log(value) vérifie que les données du serveur on bien été récupérées et voit ce qu'elles contiennent.
+- Un console.log(err) est lancé si la connexion au serveur ne s'est pas faite et que les données n'ont pas été récupérées correctement.</t>
+  </si>
+  <si>
+    <t>14 à 32</t>
+  </si>
+  <si>
+    <t>Vérification à l'affichage de la page index.html que l'on retrouve bien les bonnes informations sur les ours en peluches affiché dans la console par le console.log(value).</t>
+  </si>
+  <si>
+    <t>Le code html ne s'affiche pas correctement au chargement de la page et les différentes cartes présentant les ours en peluches n'apparaissent pas.</t>
+  </si>
+  <si>
+    <t>2 à 5</t>
+  </si>
+  <si>
+    <t>15 à 122</t>
+  </si>
+  <si>
+    <t>23 à 55</t>
+  </si>
+  <si>
+    <t>69 à 74</t>
+  </si>
+  <si>
+    <t>76 à 81</t>
+  </si>
+  <si>
+    <t>89 à 120</t>
+  </si>
+  <si>
+    <t>Le code html ne s'affiche pas correctement au chargement de la page et les informations présentant l'ours n'apparaissent pas ou ne correspondent pas à l'ours choisi.</t>
+  </si>
+  <si>
+    <t>Vérification à l'affichage de la page infos.html que l'on retrouve bien les bonnes informations affiché dans la console grâce au console.log(infos).</t>
   </si>
 </sst>
 </file>
@@ -374,7 +458,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -424,8 +508,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,8 +564,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="75">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -480,6 +599,19 @@
     <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -504,6 +636,19 @@
     <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,8 +860,8 @@
   <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -737,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -769,12 +914,12 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" customHeight="1">
+    <row r="2" spans="1:26" ht="12" customHeight="1">
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="61.5" customHeight="1">
+    <row r="3" spans="1:26" ht="108">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -787,59 +932,71 @@
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
+      <c r="E3" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1">
@@ -847,75 +1004,79 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="108">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="84">
       <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="96">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="53" customHeight="1">
@@ -923,19 +1084,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="53" customHeight="1">
@@ -943,19 +1104,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="84">
@@ -963,19 +1124,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="84">
@@ -983,19 +1144,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="84">
@@ -1003,19 +1164,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="84">
@@ -1023,19 +1184,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="84">
@@ -1043,19 +1204,19 @@
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="168">
@@ -1063,19 +1224,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84">
@@ -1083,19 +1244,19 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="48">
@@ -1103,39 +1264,39 @@
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="84">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="120">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60">
@@ -1143,70 +1304,120 @@
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="61.5" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="61.5" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="61.5" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="B25" s="4">
+        <v>33</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="61.5" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="B26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="61.5" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="B27" s="4">
+        <v>73</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="61.5" customHeight="1">
       <c r="D28" s="3"/>

</xml_diff>